<commit_message>
Ternary and binary combined
</commit_message>
<xml_diff>
--- a/program_data/table_coordinates.xlsx
+++ b/program_data/table_coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danila/Documents/GitHub/structure-type-explorer/program_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9F2DDD-343C-1448-8E18-BB2388044EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34A29FA-54C9-5F4B-A100-2D40DC88ED62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="29400" windowHeight="18380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21460" yWindow="16480" windowWidth="28620" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classic_table" sheetId="1" r:id="rId1"/>
@@ -5935,8 +5935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED1D4B8-1522-9649-A7E0-0F5DF91C083B}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5969,7 +5969,7 @@
         <v>0.3840727687462267</v>
       </c>
       <c r="D2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5983,7 +5983,7 @@
         <v>1.959752588762248</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6025,7 +6025,7 @@
         <v>0.28688190468407609</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6039,7 +6039,7 @@
         <v>3.323516009024357</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6053,7 +6053,7 @@
         <v>4.1438693669298843</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6067,7 +6067,7 @@
         <v>5.0548102758975961</v>
       </c>
       <c r="D9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6081,7 +6081,7 @@
         <v>7.5268028062553034</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6095,7 +6095,7 @@
         <v>4.2455852294283902</v>
       </c>
       <c r="D11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6165,7 +6165,7 @@
         <v>1.310502241690209</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -6179,7 +6179,7 @@
         <v>2.7391672058275551</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6193,7 +6193,7 @@
         <v>4.226696383573759</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6207,7 +6207,7 @@
         <v>2.165279704068849</v>
       </c>
       <c r="D19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6221,7 +6221,7 @@
         <v>-10.31866110902441</v>
       </c>
       <c r="D20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6445,7 +6445,7 @@
         <v>4.5865004392198117</v>
       </c>
       <c r="D36" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -6473,7 +6473,7 @@
         <v>-9.7860488260661782</v>
       </c>
       <c r="D38" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -6725,7 +6725,7 @@
         <v>-9.1573717490301565</v>
       </c>
       <c r="D56" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -8376,7 +8376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98692C51-5CD2-C944-A17E-70DBFED0FF01}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bugs with fixed_elements
</commit_message>
<xml_diff>
--- a/program_data/table_coordinates.xlsx
+++ b/program_data/table_coordinates.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danila/Documents/GitHub/structure-type-explorer/program_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34A29FA-54C9-5F4B-A100-2D40DC88ED62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAFB5C1-8B73-4C42-8E5A-34DD19339947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21460" yWindow="16480" windowWidth="28620" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classic_table" sheetId="1" r:id="rId1"/>
     <sheet name="long_table" sheetId="2" r:id="rId2"/>
     <sheet name="separated_table" sheetId="3" r:id="rId3"/>
     <sheet name="PCA_plot" sheetId="5" r:id="rId4"/>
-    <sheet name="PCA_new_plot" sheetId="6" r:id="rId5"/>
-    <sheet name="PCA_last_plot" sheetId="7" r:id="rId6"/>
+    <sheet name="PCAspecial_plot" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="122">
   <si>
     <t>Symbol</t>
   </si>
@@ -410,7 +409,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,12 +433,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -472,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -502,26 +495,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,9 +536,6 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5935,8 +5910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED1D4B8-1522-9649-A7E0-0F5DF91C083B}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5969,7 +5944,7 @@
         <v>0.3840727687462267</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5983,7 +5958,7 @@
         <v>1.959752588762248</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6025,7 +6000,7 @@
         <v>0.28688190468407609</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6039,7 +6014,7 @@
         <v>3.323516009024357</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6053,7 +6028,7 @@
         <v>4.1438693669298843</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6067,7 +6042,7 @@
         <v>5.0548102758975961</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6081,7 +6056,7 @@
         <v>7.5268028062553034</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6095,7 +6070,7 @@
         <v>4.2455852294283902</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6165,7 +6140,7 @@
         <v>1.310502241690209</v>
       </c>
       <c r="D16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -6179,7 +6154,7 @@
         <v>2.7391672058275551</v>
       </c>
       <c r="D17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6193,7 +6168,7 @@
         <v>4.226696383573759</v>
       </c>
       <c r="D18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6207,7 +6182,7 @@
         <v>2.165279704068849</v>
       </c>
       <c r="D19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6221,7 +6196,7 @@
         <v>-10.31866110902441</v>
       </c>
       <c r="D20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6445,7 +6420,7 @@
         <v>4.5865004392198117</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -6473,7 +6448,7 @@
         <v>-9.7860488260661782</v>
       </c>
       <c r="D38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -6725,7 +6700,7 @@
         <v>-9.1573717490301565</v>
       </c>
       <c r="D56" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -7157,23 +7132,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FC8555-FE1C-C74A-B0E6-6A2E3129A113}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7182,12 +7157,12 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>9.3032441935909507</v>
+        <v>-9.6007176784744033</v>
       </c>
       <c r="C2">
-        <v>0.49212574794481428</v>
-      </c>
-      <c r="D2">
+        <v>0.3840727687462267</v>
+      </c>
+      <c r="D2" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7196,12 +7171,12 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>9.8339917680679108</v>
+        <v>-10.03851471145251</v>
       </c>
       <c r="C3">
-        <v>3.7405569247935189</v>
-      </c>
-      <c r="D3">
+        <v>1.959752588762248</v>
+      </c>
+      <c r="D3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7210,12 +7185,12 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>4.8621608837683512</v>
+        <v>-3.8618582701769322</v>
       </c>
       <c r="C4">
-        <v>-5.4629454288289896</v>
-      </c>
-      <c r="D4">
+        <v>-7.3094862177148743</v>
+      </c>
+      <c r="D4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7224,12 +7199,12 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>5.9308505747261373</v>
+        <v>-5.700042507672431</v>
       </c>
       <c r="C5">
-        <v>-2.5142224419421888</v>
-      </c>
-      <c r="D5">
+        <v>-2.285397206973077</v>
+      </c>
+      <c r="D5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7238,13 +7213,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>6.4634701445059486</v>
+        <v>-6.8482891281603733</v>
       </c>
       <c r="C6">
-        <v>-0.47100963773213422</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>0.28688190468407609</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -7252,13 +7227,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>6.9391478520192651</v>
+        <v>-7.5943292863756948</v>
       </c>
       <c r="C7">
-        <v>0.9779944760307413</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>3.323516009024357</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -7266,13 +7241,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>8.3752438367972175</v>
+        <v>-9.756485369636021</v>
       </c>
       <c r="C8">
-        <v>3.2887124609404328</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>4.1438693669298843</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7280,13 +7255,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>8.8118551860533749</v>
+        <v>-10.530399564611921</v>
       </c>
       <c r="C9">
-        <v>4.3865361234411253</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>5.0548102758975961</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7294,12 +7269,12 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>9.345902701734822</v>
+        <v>-11.90463201759635</v>
       </c>
       <c r="C10">
-        <v>5.8998482451751979</v>
-      </c>
-      <c r="D10">
+        <v>7.5268028062553034</v>
+      </c>
+      <c r="D10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7308,12 +7283,12 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>9.5647829727098284</v>
+        <v>-10.25715780254683</v>
       </c>
       <c r="C11">
-        <v>6.7004663492131984</v>
-      </c>
-      <c r="D11">
+        <v>4.2455852294283902</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7322,12 +7297,12 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>3.6738646017595391</v>
+        <v>-2.442535348986882</v>
       </c>
       <c r="C12">
-        <v>-6.1797314801226824</v>
-      </c>
-      <c r="D12">
+        <v>-8.4002347363848742</v>
+      </c>
+      <c r="D12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7336,12 +7311,12 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>4.73596555367227</v>
+        <v>-4.104359868775517</v>
       </c>
       <c r="C13">
-        <v>-3.4080832990501482</v>
-      </c>
-      <c r="D13">
+        <v>-4.8238739853016881</v>
+      </c>
+      <c r="D13" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7350,13 +7325,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>5.1705137801438141</v>
+        <v>-4.791260107552886</v>
       </c>
       <c r="C14">
-        <v>-1.967818023973614</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>-2.745837853400495</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -7364,13 +7339,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>6.0312062480452306</v>
+        <v>-6.1218531830812353</v>
       </c>
       <c r="C15">
-        <v>1.774381838597253E-2</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>0.34770080834475298</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -7378,13 +7353,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>6.5602611915533107</v>
+        <v>-7.1244703959441367</v>
       </c>
       <c r="C16">
-        <v>1.6639591792103561</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>1.310502241690209</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -7392,13 +7367,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>6.9142361171211659</v>
+        <v>-8.2164589071446468</v>
       </c>
       <c r="C17">
-        <v>2.617240300632818</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>2.7391672058275551</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -7406,12 +7381,12 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>7.4778564041065776</v>
+        <v>-9.0710010271642343</v>
       </c>
       <c r="C18">
-        <v>3.963996395612313</v>
-      </c>
-      <c r="D18">
+        <v>4.226696383573759</v>
+      </c>
+      <c r="D18" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7420,12 +7395,12 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>7.5356283703946074</v>
+        <v>-7.9643255718694137</v>
       </c>
       <c r="C19">
-        <v>4.6017219524251516</v>
-      </c>
-      <c r="D19">
+        <v>2.165279704068849</v>
+      </c>
+      <c r="D19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7434,12 +7409,12 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>2.0602733907929371</v>
+        <v>-0.39890524127189358</v>
       </c>
       <c r="C20">
-        <v>-7.5068364086892716</v>
-      </c>
-      <c r="D20">
+        <v>-10.31866110902441</v>
+      </c>
+      <c r="D20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7448,12 +7423,12 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>2.7829188991498439</v>
+        <v>-1.5322330776471851</v>
       </c>
       <c r="C21">
-        <v>-5.2736661006339354</v>
-      </c>
-      <c r="D21">
+        <v>-7.4548424668124742</v>
+      </c>
+      <c r="D21" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7462,13 +7437,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>2.6356441630247631</v>
+        <v>-1.7616317308007201</v>
       </c>
       <c r="C22">
-        <v>-4.588720962089301</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
+        <v>-5.2021463721741004</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -7476,13 +7451,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>2.8504953479451909</v>
+        <v>-2.178666928476908</v>
       </c>
       <c r="C23">
-        <v>-3.525508727011792</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
+        <v>-3.5688876670574698</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -7490,13 +7465,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>2.913002748257342</v>
+        <v>-2.405796764632818</v>
       </c>
       <c r="C24">
-        <v>-3.002489826791503</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>-2.5149425499581062</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -7504,13 +7479,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>2.955738652435715</v>
+        <v>-2.5442123934295928</v>
       </c>
       <c r="C25">
-        <v>-3.0071595612961608</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+        <v>-2.2640403739286268</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -7518,13 +7493,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>3.1932397066077511</v>
+        <v>-2.8711158372048482</v>
       </c>
       <c r="C26">
-        <v>-1.9056199901390121</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>-1.917141402722732</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -7532,13 +7507,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>3.1170568956078482</v>
+        <v>-2.8378506952298328</v>
       </c>
       <c r="C27">
-        <v>-1.5680027156900009</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>-0.87089002190007192</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -7546,13 +7521,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>2.9968591485214819</v>
+        <v>-2.7841377456617908</v>
       </c>
       <c r="C28">
-        <v>-1.4687547341837051</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+        <v>-0.59421397373808726</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -7560,12 +7535,12 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>2.996369779293611</v>
+        <v>-2.8535157429982978</v>
       </c>
       <c r="C29">
-        <v>-1.192805291999115</v>
-      </c>
-      <c r="D29">
+        <v>-0.2311168196998212</v>
+      </c>
+      <c r="D29" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7574,12 +7549,12 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>2.946411055001295</v>
+        <v>-2.704101612747333</v>
       </c>
       <c r="C30">
-        <v>-1.607209791981727</v>
-      </c>
-      <c r="D30">
+        <v>-1.152430609056887</v>
+      </c>
+      <c r="D30" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7588,12 +7563,12 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>3.264739054872881</v>
+        <v>-3.0777857141853251</v>
       </c>
       <c r="C31">
-        <v>-0.57353380523392916</v>
-      </c>
-      <c r="D31">
+        <v>-1.291577912194904</v>
+      </c>
+      <c r="D31" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7602,13 +7577,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>3.380898087790051</v>
+        <v>-3.1434530527113069</v>
       </c>
       <c r="C32">
-        <v>-0.22640003604928929</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
+        <v>-1.085578033054067</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -7616,13 +7591,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>3.6361595395942672</v>
+        <v>-3.6921904647085881</v>
       </c>
       <c r="C33">
-        <v>1.0001008613960689</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+        <v>1.4785728268109559</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -7630,13 +7605,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>4.2643730011875958</v>
+        <v>-4.7075180919898942</v>
       </c>
       <c r="C34">
-        <v>2.2937731084442441</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+        <v>1.9107799294273351</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -7644,13 +7619,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>4.7095922261359906</v>
+        <v>-5.5666305565161851</v>
       </c>
       <c r="C35">
-        <v>3.912667341515093</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+        <v>2.994299549811299</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -7658,12 +7633,12 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>5.0601831172266509</v>
+        <v>-6.399783851618265</v>
       </c>
       <c r="C36">
-        <v>5.1240682800714854</v>
-      </c>
-      <c r="D36">
+        <v>4.5865004392198117</v>
+      </c>
+      <c r="D36" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7672,12 +7647,12 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>5.1046293287281417</v>
+        <v>-5.7196952524402063</v>
       </c>
       <c r="C37">
-        <v>5.5400917293073393</v>
-      </c>
-      <c r="D37">
+        <v>3.3578349696026941</v>
+      </c>
+      <c r="D37" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7686,12 +7661,12 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>-0.22415891919703471</v>
+        <v>1.8900679298288581</v>
       </c>
       <c r="C38">
-        <v>-7.1452142806973757</v>
-      </c>
-      <c r="D38">
+        <v>-9.7860488260661782</v>
+      </c>
+      <c r="D38" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7700,12 +7675,12 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>0.46663001375578089</v>
+        <v>0.87111198678639046</v>
       </c>
       <c r="C39">
-        <v>-4.9286243547239961</v>
-      </c>
-      <c r="D39">
+        <v>-7.1501810330298587</v>
+      </c>
+      <c r="D39" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7714,13 +7689,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>0.1908646387926369</v>
+        <v>0.74996754135782073</v>
       </c>
       <c r="C40">
-        <v>-4.3705427958211969</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
+        <v>-5.0800980390394912</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -7728,13 +7703,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>0.28366431296679367</v>
+        <v>0.44313180229883092</v>
       </c>
       <c r="C41">
-        <v>-3.3910353240185001</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
+        <v>-3.2909914985913979</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -7742,13 +7717,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>0.1673985255100936</v>
+        <v>0.36981387485254452</v>
       </c>
       <c r="C42">
-        <v>-3.2364826992453279</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>-2.0447677362170609</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -7756,13 +7731,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>0.1373913077134471</v>
+        <v>0.25506863970008792</v>
       </c>
       <c r="C43">
-        <v>-2.7576947846338791</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
+        <v>-0.94499411635859498</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -7770,12 +7745,12 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>0.1087275495348822</v>
+        <v>0.26141970072967458</v>
       </c>
       <c r="C44">
-        <v>-1.770730064889672</v>
-      </c>
-      <c r="D44">
+        <v>-0.45484575373493058</v>
+      </c>
+      <c r="D44" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7784,13 +7759,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>0.17733048670365559</v>
+        <v>0.1015335316699135</v>
       </c>
       <c r="C45">
-        <v>-1.71317597459019</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
+        <v>0.58693947158623216</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -7798,12 +7773,12 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>0.14665042879703771</v>
+        <v>4.9157781296857592E-2</v>
       </c>
       <c r="C46">
-        <v>-1.476537197057306</v>
-      </c>
-      <c r="D46">
+        <v>0.42573833995491628</v>
+      </c>
+      <c r="D46" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7812,12 +7787,12 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>0.97231419476494851</v>
+        <v>-1.174859161979968</v>
       </c>
       <c r="C47">
-        <v>-0.16305140346168159</v>
-      </c>
-      <c r="D47">
+        <v>1.316758282135601</v>
+      </c>
+      <c r="D47" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7826,13 +7801,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>0.3481615300321842</v>
+        <v>-0.13813209120656469</v>
       </c>
       <c r="C48">
-        <v>-0.93524537930778961</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
+        <v>-0.97785629110707939</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -7840,12 +7815,12 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>0.60330861815250858</v>
+        <v>-0.36113472288601989</v>
       </c>
       <c r="C49">
-        <v>7.1286957728409678E-2</v>
-      </c>
-      <c r="D49">
+        <v>-1.0027580473074731</v>
+      </c>
+      <c r="D49" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7854,13 +7829,13 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>0.49699850270294837</v>
+        <v>-0.20996014115262221</v>
       </c>
       <c r="C50">
-        <v>0.36838621420544282</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
+        <v>-0.83632346301749327</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -7868,12 +7843,12 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>0.57182064584314951</v>
+        <v>-0.65898629663286767</v>
       </c>
       <c r="C51">
-        <v>1.251673592119888</v>
-      </c>
-      <c r="D51">
+        <v>0.54551037753703424</v>
+      </c>
+      <c r="D51" s="4">
         <v>1</v>
       </c>
     </row>
@@ -7882,13 +7857,13 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>1.131683087264328</v>
+        <v>-1.535116558541286</v>
       </c>
       <c r="C52">
-        <v>2.8064671939107062</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
+        <v>2.111425898032302</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -7896,13 +7871,13 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>1.3618402970935091</v>
+        <v>-2.058527064038099</v>
       </c>
       <c r="C53">
-        <v>4.2804850788001314</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
+        <v>3.1940805724298929</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -7910,12 +7885,12 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>1.678719795268568</v>
+        <v>-2.8804190779937269</v>
       </c>
       <c r="C54">
-        <v>5.5203004064588876</v>
-      </c>
-      <c r="D54">
+        <v>4.668722097505233</v>
+      </c>
+      <c r="D54" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7924,12 +7899,12 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>1.9964317476406701</v>
+        <v>-2.5796903323415341</v>
       </c>
       <c r="C55">
-        <v>5.778129992885618</v>
-      </c>
-      <c r="D55">
+        <v>3.8651132172414249</v>
+      </c>
+      <c r="D55" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7938,12 +7913,12 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>-3.641609972365357</v>
+        <v>5.1245458440697087</v>
       </c>
       <c r="C56">
-        <v>-6.7993149233546086</v>
-      </c>
-      <c r="D56">
+        <v>-9.1573717490301565</v>
+      </c>
+      <c r="D56" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7952,12 +7927,12 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>-2.891958683208355</v>
+        <v>3.9104461570002891</v>
       </c>
       <c r="C57">
-        <v>-4.3003088561499636</v>
-      </c>
-      <c r="D57">
+        <v>-6.0221791890055734</v>
+      </c>
+      <c r="D57" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7966,13 +7941,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>-3.0369485617042788</v>
+        <v>3.7242657863294188</v>
       </c>
       <c r="C58">
-        <v>-3.4060243798141632</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>-3.9077370047835029</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -7980,13 +7955,13 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>-3.403305820141159</v>
+        <v>3.9073704330696288</v>
       </c>
       <c r="C59">
-        <v>-2.8504831696372301</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
+        <v>-2.9561404118901069</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -7994,13 +7969,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>-3.739810903388237</v>
+        <v>4.2538122143583417</v>
       </c>
       <c r="C60">
-        <v>-3.0342146888729729</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
+        <v>-3.2181233859156988</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -8008,13 +7983,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>-3.9100311050621359</v>
+        <v>4.3512030695602943</v>
       </c>
       <c r="C61">
-        <v>-2.5756265133731229</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
+        <v>-2.837116462126942</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -8022,12 +7997,12 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>-3.6995165858125318</v>
+        <v>4.0458836598412926</v>
       </c>
       <c r="C62">
-        <v>-2.6882112185255029</v>
-      </c>
-      <c r="D62">
+        <v>-2.7038723289170798</v>
+      </c>
+      <c r="D62" s="4">
         <v>0</v>
       </c>
     </row>
@@ -8036,13 +8011,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>-4.2872067904107913</v>
+        <v>4.7621533918426184</v>
       </c>
       <c r="C63">
-        <v>-2.202679961898252</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
+        <v>-2.7149605601969129</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -8050,13 +8025,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>-4.4812443602040846</v>
+        <v>4.9427979724280613</v>
       </c>
       <c r="C64">
-        <v>-2.001596733905922</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+        <v>-2.8418815250961051</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -8064,13 +8039,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>-5.0638308952198621</v>
+        <v>5.5683493435897766</v>
       </c>
       <c r="C65">
-        <v>-1.913578321184062</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
+        <v>-2.076788855718843</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -8078,13 +8053,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>-5.1744201532482803</v>
+        <v>5.4686254770843696</v>
       </c>
       <c r="C66">
-        <v>-1.5013309970993849</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
+        <v>-1.4117208388909741</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -8092,13 +8067,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>-5.3072770075596214</v>
+        <v>5.5600096535638821</v>
       </c>
       <c r="C67">
-        <v>-1.1623295400109599</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
+        <v>-1.22971393295469</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -8106,13 +8081,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>-5.6024680502601161</v>
+        <v>5.8156339536878408</v>
       </c>
       <c r="C68">
-        <v>-0.9507104079248514</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
+        <v>-0.90947359676612483</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -8120,13 +8095,13 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>-5.9099861376737683</v>
+        <v>6.0884702992835518</v>
       </c>
       <c r="C69">
-        <v>-0.69742629637596731</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
+        <v>-0.55928994301412716</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -8134,13 +8109,13 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>-6.0768380910355448</v>
+        <v>6.1905465664419523</v>
       </c>
       <c r="C70">
-        <v>-0.28563724682429148</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+        <v>-0.3219245420280703</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -8148,13 +8123,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>-6.1942076100995394</v>
+        <v>6.3570012480944929</v>
       </c>
       <c r="C71">
-        <v>-1.9204165720835709E-2</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+        <v>-0.74144383752730925</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -8162,13 +8137,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>-6.808272192871561</v>
+        <v>6.9258161229608177</v>
       </c>
       <c r="C72">
-        <v>-0.1537132862344408</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
+        <v>0.17670341106979209</v>
+      </c>
+      <c r="D72" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -8176,13 +8151,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>-7.0286940118123331</v>
+        <v>6.9864274000929374</v>
       </c>
       <c r="C73">
-        <v>0.72602937488646568</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
+        <v>1.8536559104857171</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -8190,13 +8165,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>-7.4198430860576252</v>
+        <v>7.2277722180380746</v>
       </c>
       <c r="C74">
-        <v>1.3924656248459051</v>
-      </c>
-      <c r="D74">
-        <v>1</v>
+        <v>3.4454331628366242</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -8204,13 +8179,13 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>-7.7108772961685226</v>
+        <v>7.3663619088819337</v>
       </c>
       <c r="C75">
-        <v>1.9274254160600219</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
+        <v>5.3454185091580966</v>
+      </c>
+      <c r="D75" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -8218,13 +8193,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>-7.8538701802648712</v>
+        <v>7.4939010446863428</v>
       </c>
       <c r="C76">
-        <v>2.59415923056173</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
+        <v>5.7973185206801547</v>
+      </c>
+      <c r="D76" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -8232,13 +8207,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>-8.1035400364709673</v>
+        <v>7.5553171753878976</v>
       </c>
       <c r="C77">
-        <v>3.3937549196271668</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
+        <v>6.8393714880092693</v>
+      </c>
+      <c r="D77" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -8246,13 +8221,13 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>-8.0933486588937722</v>
+        <v>7.4894832679092662</v>
       </c>
       <c r="C78">
-        <v>3.740018504584012</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+        <v>6.9948717089478434</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -8260,13 +8235,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>-8.15447854312408</v>
+        <v>7.3986506605191238</v>
       </c>
       <c r="C79">
-        <v>3.9456883438060508</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
+        <v>6.3405786013805168</v>
+      </c>
+      <c r="D79" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -8274,13 +8249,13 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>-8.2916164988768912</v>
+        <v>7.3812353676690616</v>
       </c>
       <c r="C80">
-        <v>4.43723461513129</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
+        <v>6.3371657921438338</v>
+      </c>
+      <c r="D80" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -8288,12 +8263,12 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>-7.7263559319744619</v>
+        <v>7.0807067553489391</v>
       </c>
       <c r="C81">
-        <v>5.4466641071859074</v>
-      </c>
-      <c r="D81">
+        <v>5.1204884773525281</v>
+      </c>
+      <c r="D81" s="4">
         <v>0</v>
       </c>
     </row>
@@ -8302,13 +8277,13 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>-7.9420729966697081</v>
+        <v>7.4953409629858339</v>
       </c>
       <c r="C82">
-        <v>4.9391299632003101</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
+        <v>4.0135093534706892</v>
+      </c>
+      <c r="D82" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -8316,13 +8291,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>-7.9827207911676332</v>
+        <v>7.2807962375040578</v>
       </c>
       <c r="C83">
-        <v>5.7646158832167034</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>5.049259182801924</v>
+      </c>
+      <c r="D83" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -8330,13 +8305,13 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>-7.9501368105055601</v>
+        <v>7.0585909666363378</v>
       </c>
       <c r="C84">
-        <v>6.4677797087519249</v>
-      </c>
-      <c r="D84">
-        <v>1</v>
+        <v>6.0145753971219316</v>
+      </c>
+      <c r="D84" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -8344,13 +8319,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>-12.43073539736838</v>
+        <v>12.25876957222793</v>
       </c>
       <c r="C85">
-        <v>0.76718232439403422</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
+        <v>2.4171397873965459</v>
+      </c>
+      <c r="D85" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -8358,1022 +8333,13 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>-13.097320126663771</v>
+        <v>12.643183428651049</v>
       </c>
       <c r="C86">
-        <v>2.040762481891464</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98692C51-5CD2-C944-A17E-70DBFED0FF01}">
-  <dimension ref="A1:D71"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>-4.4340097192537584</v>
-      </c>
-      <c r="C2">
-        <v>-4.6042680807322194</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>-0.21763945631473569</v>
-      </c>
-      <c r="C3">
-        <v>-4.3345119930368394</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2.0685215834095332</v>
-      </c>
-      <c r="C4">
-        <v>-4.2118665949167839</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>5.7812440511375698</v>
-      </c>
-      <c r="C5">
-        <v>-4.110946113319633</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>-4.676906601110649</v>
-      </c>
-      <c r="C6">
-        <v>-2.140532490645227</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>-2.3115169033767469</v>
-      </c>
-      <c r="C7">
-        <v>-2.5603593895900252</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>-0.80341507060498329</v>
-      </c>
-      <c r="C8">
-        <v>-2.6087092588910679</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>1.592644139501119</v>
-      </c>
-      <c r="C9">
-        <v>-3.1614146976444251</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <v>2.1059701316598041</v>
-      </c>
-      <c r="C10">
-        <v>-3.5284204865321862</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>2.7408759215942</v>
-      </c>
-      <c r="C11">
-        <v>-4.2531667720325252</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>-5.5434772581691218</v>
-      </c>
-      <c r="C12">
-        <v>-1.2106619220403769</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13">
-        <v>-3.1438031910214379</v>
-      </c>
-      <c r="C13">
-        <v>-1.2929213986086401</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14">
-        <v>-1.7033208350667319</v>
-      </c>
-      <c r="C14">
-        <v>-1.1535142479952669</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15">
-        <v>-0.1552917695663274</v>
-      </c>
-      <c r="C15">
-        <v>-1.230794616295376</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>0.79741077026659457</v>
-      </c>
-      <c r="C16">
-        <v>-1.014379394710694</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17">
-        <v>0.9355626293990541</v>
-      </c>
-      <c r="C17">
-        <v>-0.93586534435428304</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18">
-        <v>0.96251058074694751</v>
-      </c>
-      <c r="C18">
-        <v>-1.285996436117181</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19">
-        <v>1.393444701111104</v>
-      </c>
-      <c r="C19">
-        <v>-0.82384723693201478</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20">
-        <v>1.574789000747904</v>
-      </c>
-      <c r="C20">
-        <v>-0.92757663237685284</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21">
-        <v>1.4959776810230689</v>
-      </c>
-      <c r="C21">
-        <v>-1.0024631442866749</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22">
-        <v>0.37710340018802052</v>
-      </c>
-      <c r="C22">
-        <v>-0.87335281474201343</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23">
-        <v>-0.62823634531147021</v>
-      </c>
-      <c r="C23">
-        <v>-1.3023434422281619</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24">
-        <v>-0.43523294565442339</v>
-      </c>
-      <c r="C24">
-        <v>-1.715584951132314</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25">
-        <v>1.780247570251603</v>
-      </c>
-      <c r="C25">
-        <v>-1.7398309030739401</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26">
-        <v>1.977877502574015</v>
-      </c>
-      <c r="C26">
-        <v>-1.663281083887123</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27">
-        <v>2.912970451741014</v>
-      </c>
-      <c r="C27">
-        <v>-2.387520565875811</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28">
-        <v>-5.4072087325876952</v>
-      </c>
-      <c r="C28">
-        <v>7.790431391479594E-3</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29">
-        <v>-2.9328348180037902</v>
-      </c>
-      <c r="C29">
-        <v>-0.54473508092224421</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30">
-        <v>-2.048778461356338</v>
-      </c>
-      <c r="C30">
-        <v>0.13942115873913791</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31">
-        <v>-0.324056021843108</v>
-      </c>
-      <c r="C31">
-        <v>0.13181964570263061</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32">
-        <v>1.168266455326415</v>
-      </c>
-      <c r="C32">
-        <v>0.48577470585835719</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33">
-        <v>2.3151263912435862</v>
-      </c>
-      <c r="C33">
-        <v>0.5696301205389922</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34">
-        <v>3.032732232317799</v>
-      </c>
-      <c r="C34">
-        <v>0.42409488639325887</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35">
-        <v>2.803275176915581</v>
-      </c>
-      <c r="C35">
-        <v>0.2724710285838941</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36">
-        <v>1.8847130847154441</v>
-      </c>
-      <c r="C36">
-        <v>-0.46576536516442041</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37">
-        <v>1.6088715580944719E-2</v>
-      </c>
-      <c r="C37">
-        <v>0.21612105931330139</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38">
-        <v>-0.95947365991000022</v>
-      </c>
-      <c r="C38">
-        <v>-0.1090058207320268</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39">
-        <v>-1.1830342070841151</v>
-      </c>
-      <c r="C39">
-        <v>4.9517391379647092E-2</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40">
-        <v>0.54437671249270514</v>
-      </c>
-      <c r="C40">
-        <v>-0.38782505905288212</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41">
-        <v>1.312896933961728</v>
-      </c>
-      <c r="C41">
-        <v>-0.42952121267885451</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42">
-        <v>2.3138893065433939</v>
-      </c>
-      <c r="C42">
-        <v>-0.93243483473078204</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43">
-        <v>-5.7139715041573327</v>
-      </c>
-      <c r="C43">
-        <v>0.95201541504974385</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44">
-        <v>-4.0972946122254958</v>
-      </c>
-      <c r="C44">
-        <v>1.0790992955458329</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45">
-        <v>-2.4705926396567972</v>
-      </c>
-      <c r="C45">
-        <v>1.057600059295124</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46">
-        <v>-2.1481512207687872</v>
-      </c>
-      <c r="C46">
-        <v>1.006860453680603</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47">
-        <v>-2.0375573161647118</v>
-      </c>
-      <c r="C47">
-        <v>1.2472114363060709</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48">
-        <v>-1.845131410723162</v>
-      </c>
-      <c r="C48">
-        <v>1.373141044638736</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49">
-        <v>-1.761425365655771</v>
-      </c>
-      <c r="C49">
-        <v>1.6149543677128659</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50">
-        <v>-2.653172873097184</v>
-      </c>
-      <c r="C50">
-        <v>2.0620262753798748</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51">
-        <v>-1.1652409754601381</v>
-      </c>
-      <c r="C51">
-        <v>2.0313552801159669</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52">
-        <v>-1.187470652394844</v>
-      </c>
-      <c r="C52">
-        <v>1.8904925603383571</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53">
-        <v>-1.321535678270831</v>
-      </c>
-      <c r="C53">
-        <v>1.8058679469582291</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54">
-        <v>-1.2340547559642261</v>
-      </c>
-      <c r="C54">
-        <v>1.782867189459018</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55">
-        <v>-1.1587223018763171</v>
-      </c>
-      <c r="C55">
-        <v>1.755119001121404</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56">
-        <v>-1.273501382985702</v>
-      </c>
-      <c r="C56">
-        <v>1.6046138252525759</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57">
-        <v>-2.1175967651463372</v>
-      </c>
-      <c r="C57">
-        <v>1.689577175848014</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58">
-        <v>-1.4102624462966951</v>
-      </c>
-      <c r="C58">
-        <v>2.0867684138778548</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59">
-        <v>0.69854526224384761</v>
-      </c>
-      <c r="C59">
-        <v>2.2922015703552052</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60">
-        <v>2.3616771381756179</v>
-      </c>
-      <c r="C60">
-        <v>2.8459738894839699</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61">
-        <v>4.0705678431736194</v>
-      </c>
-      <c r="C61">
-        <v>3.0900231755991872</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62">
-        <v>4.2071776563328331</v>
-      </c>
-      <c r="C62">
-        <v>2.6749083247664291</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63">
-        <v>4.6304448313407756</v>
-      </c>
-      <c r="C63">
-        <v>3.101126805827588</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64">
-        <v>4.2320126493785857</v>
-      </c>
-      <c r="C64">
-        <v>2.4681575843999699</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65">
-        <v>3.2914427573796901</v>
-      </c>
-      <c r="C65">
-        <v>2.0545141704264189</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66">
-        <v>2.180528616947258</v>
-      </c>
-      <c r="C66">
-        <v>2.3545797614628921</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67">
-        <v>-0.58419073628055918</v>
-      </c>
-      <c r="C67">
-        <v>1.969667643563513</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68">
-        <v>0.537755362593063</v>
-      </c>
-      <c r="C68">
-        <v>2.0957241269920548</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>86</v>
-      </c>
-      <c r="B69">
-        <v>1.1779437541118141</v>
-      </c>
-      <c r="C69">
-        <v>1.3566504944953699</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70">
-        <v>-0.60201556041949245</v>
-      </c>
-      <c r="C70">
-        <v>2.7364936102820931</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71">
-        <v>0.41351319765356298</v>
-      </c>
-      <c r="C71">
-        <v>2.567186059143209</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+        <v>4.7074997120451298</v>
+      </c>
+      <c r="D86" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>